<commit_message>
Pc's back, so time to reorganize stuff
</commit_message>
<xml_diff>
--- a/Data Preprocessing/1 - Excel/introduction to excel - class example.xlsx
+++ b/Data Preprocessing/1 - Excel/introduction to excel - class example.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\meng4\Desktop\NOVA IMS PRACTICAL CLASSES\Data Preprocessing\1 - Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\meng4\Desktop\Nova IMS Pratical Classes\Data Preprocessing\1 - Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{331F98F7-E73E-4233-BA96-9AC622949A52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1DCA3D2-4A0E-49E4-8820-AF0DA0FC4409}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1ST DEMO" sheetId="1" r:id="rId1"/>
@@ -34,9 +34,8 @@
   </definedNames>
   <calcPr calcId="191028"/>
   <pivotCaches>
-    <pivotCache cacheId="5" r:id="rId8"/>
+    <pivotCache cacheId="0" r:id="rId8"/>
   </pivotCaches>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -57,7 +56,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -407,6 +406,3204 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="it-IT"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Company A - LISBON'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Sales</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Company A - LISBON'!$A$2:$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Kitchen</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Bedroom</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Eletronics</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Company A - LISBON'!$B$2:$B$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>123000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>560000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-AA39-4B09-A906-DAA416C74E39}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1219797663"/>
+        <c:axId val="1219804863"/>
+      </c:barChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Company A - LISBON'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Quantity</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Company A - LISBON'!$A$2:$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Kitchen</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Bedroom</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Eletronics</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Company A - LISBON'!$C$2:$C$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>340</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>145</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-AA39-4B09-A906-DAA416C74E39}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="1219801503"/>
+        <c:axId val="1219799103"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1219797663"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1219804863"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1219804863"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1219797663"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1219799103"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1219801503"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="1219801503"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="1219799103"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="it-IT"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="it-IT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="it-IT"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Company A - PORTO'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Sales</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Company A - PORTO'!$A$2:$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Kitchen</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Bedroom</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Eletronics</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Living room</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Bathroom</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Company A - PORTO'!$B$2:$B$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>45000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>345000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>125000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>349000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8F74-4DF2-88A7-9AC31AC6C10B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1218632143"/>
+        <c:axId val="1218625423"/>
+      </c:barChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Company A - PORTO'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Quantity</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Company A - PORTO'!$A$2:$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Kitchen</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Bedroom</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Eletronics</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Living room</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Bathroom</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Company A - PORTO'!$C$2:$C$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>280</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>140</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-8F74-4DF2-88A7-9AC31AC6C10B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="1218632623"/>
+        <c:axId val="1218636463"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1218632143"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1218625423"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1218625423"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1218632143"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1218636463"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1218632623"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="1218632623"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="1218636463"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="it-IT"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="it-IT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="it-IT"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Company A - Madrid'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Sales</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Company A - Madrid'!$A$2:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Kitchen</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Bedroom</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Eletronics</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Living room</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Bathroom</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Garden</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Company A - Madrid'!$B$2:$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>750000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>498000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>639000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>273000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>560000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1790500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-95EA-4C08-BB3E-50F22B402DBC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1218644143"/>
+        <c:axId val="1218633583"/>
+      </c:barChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Company A - Madrid'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Quantity</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Company A - Madrid'!$A$2:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Kitchen</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Bedroom</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Eletronics</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Living room</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Bathroom</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Garden</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Company A - Madrid'!$C$2:$C$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>650</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1050</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>580</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>890</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-95EA-4C08-BB3E-50F22B402DBC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="1218638863"/>
+        <c:axId val="1218630703"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1218644143"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1218633583"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1218633583"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1218644143"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1218630703"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1218638863"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="1218638863"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="1218630703"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="it-IT"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="it-IT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>396240</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>41910</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>91440</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>41910</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{97963812-5231-27D0-E325-7B05E5D8A96F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>396240</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>91440</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AA12A31F-CC71-68E1-2E80-7FF9B9C02FA3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1792</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>897</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>306592</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>896</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CC5B2E84-21AB-2EC2-13DF-9CCDC6555A60}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -751,7 +3948,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0BDE6FC8-A9FE-41D4-B925-275D2B498766}" name="PivotTable1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0BDE6FC8-A9FE-41D4-B925-275D2B498766}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="F18:K25" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField axis="axisCol" showAll="0">
@@ -1179,6 +4376,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView zoomScale="109" zoomScaleNormal="130" workbookViewId="0">
@@ -1420,6 +4618,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C99AE0E7-5FFA-4449-95BB-75F6D10442B6}">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView zoomScale="139" zoomScaleNormal="156" workbookViewId="0">
@@ -1476,7 +4675,7 @@
         <v>31</v>
       </c>
       <c r="B5" s="7">
-        <f t="shared" ref="B5:B10" si="0">IF(A5="summer",0,1)</f>
+        <f t="shared" ref="B5:B9" si="0">IF(A5="summer",0,1)</f>
         <v>1</v>
       </c>
       <c r="I5" s="1">
@@ -1613,6 +4812,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:M36"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="160" workbookViewId="0">
@@ -2034,6 +5234,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:K54"/>
   <sheetViews>
     <sheetView topLeftCell="B9" zoomScale="113" zoomScaleNormal="100" workbookViewId="0">
@@ -2803,10 +6004,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC6BD2CF-9510-48F7-A268-9A1D0C036819}">
+  <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C4"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2857,15 +6059,17 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D84E34B-2CAC-47E6-8A76-DDBFCD9D07DE}">
+  <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView zoomScale="85" workbookViewId="0">
+      <selection activeCell="J34" sqref="J34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2938,15 +6142,17 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{599C272A-0EB8-4A75-86CA-466AE447BF16}">
+  <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3030,5 +6236,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>